<commit_message>
Hoan thanh quan kho
</commit_message>
<xml_diff>
--- a/exportfile/tonkho.xlsx
+++ b/exportfile/tonkho.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Mã NL</t>
   </si>
@@ -72,6 +72,24 @@
   </si>
   <si>
     <t>gam</t>
+  </si>
+  <si>
+    <t>NL006</t>
+  </si>
+  <si>
+    <t>Trái Ổi</t>
+  </si>
+  <si>
+    <t>Ổi sân vườn</t>
+  </si>
+  <si>
+    <t>NL007</t>
+  </si>
+  <si>
+    <t>Tôm hùm alaska</t>
+  </si>
+  <si>
+    <t>lấy ở biển đông</t>
   </si>
 </sst>
 </file>
@@ -116,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -202,6 +220,46 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>